<commit_message>
Use US data as temporary placeholder for elec/EoTCCwTC
</commit_message>
<xml_diff>
--- a/InputData/elec/EoTCCwTC/Elasticity of TCC wrt Transmission Capacity.xlsx
+++ b/InputData/elec/EoTCCwTC/Elasticity of TCC wrt Transmission Capacity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\elec\EoTCCwTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\elec\EoTCCwTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209D8863-D868-4F2C-B5F9-C5D8AA4EA6EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-113" windowWidth="19418" windowHeight="10418"/>
+    <workbookView xWindow="4575" yWindow="-17715" windowWidth="29040" windowHeight="17265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,6 +35,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="97">
   <si>
     <t>a physical build-out of the system) and change in the Transmission</t>
   </si>
@@ -355,11 +357,14 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>The EU EPS currently uses values from the US EPS.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -405,7 +410,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,6 +429,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -438,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -462,6 +473,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,11 +789,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -856,89 +869,98 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="20"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -946,12 +968,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -1257,10 +1277,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AP19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -1706,12 +1726,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH225"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160:AH176"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -16180,14 +16198,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.499984740745262"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>